<commit_message>
Nablarch 5u18 -> 5u19へ
</commit_message>
<xml_diff>
--- a/nablarch-handson-app-web/src/test/java/com/nablarch/example/app/web/action/AuthenticationActionRequestTest.xlsx
+++ b/nablarch-handson-app-web/src/test/java/com/nablarch/example/app/web/action/AuthenticationActionRequestTest.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PJ\01.Nablarch\repo\Nablarch\Examples\nablarch-example-web\src\test\java\com\nablarch\example\app\web\action\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C398497-C610-443F-A77A-AF4D3860F07A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="16380" windowHeight="8070" tabRatio="766"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" tabRatio="766" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setUpDb" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="107">
   <si>
     <t>LIST_MAP=user</t>
     <phoneticPr fontId="2"/>
@@ -141,10 +147,6 @@
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>400</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -538,10 +540,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>index</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>5</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -579,11 +577,15 @@
     <t>303</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>403</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -843,7 +845,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準_testMenus00102Normal" xfId="1"/>
+    <cellStyle name="標準_testMenus00102Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -919,12 +921,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -966,7 +971,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -999,9 +1004,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1034,6 +1056,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1209,7 +1248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -1243,13 +1282,13 @@
     </row>
     <row r="2" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
@@ -1269,94 +1308,94 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="C5" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="D5" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="E5" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="F5" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="G5" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="H5" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="I5" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="J5" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="K5" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="L5" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="L5" s="44" t="s">
+      <c r="M5" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="N5" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="44" t="s">
+      <c r="O5" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="P5" s="44" t="s">
         <v>87</v>
-      </c>
-      <c r="P5" s="44" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="D8" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="E8" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="F8" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="G8" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="H8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="I8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="J8" s="36" t="s">
         <v>44</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -1379,10 +1418,10 @@
         <v>19</v>
       </c>
       <c r="B11" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1398,7 +1437,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV18"/>
   <sheetViews>
@@ -1725,13 +1764,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14" t="s">
@@ -1740,7 +1779,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -2271,7 +2310,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -2529,13 +2568,13 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -2793,7 +2832,7 @@
     </row>
     <row r="11" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:256" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
@@ -3082,7 +3121,7 @@
     </row>
     <row r="17" spans="1:255" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3341,7 +3380,7 @@
     </row>
     <row r="18" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3357,7 +3396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleSheetLayoutView="10" workbookViewId="0"/>
@@ -3683,13 +3722,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14" t="s">
@@ -3698,7 +3737,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -4229,7 +4268,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -4487,13 +4526,13 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -4751,7 +4790,7 @@
     </row>
     <row r="11" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:256" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
@@ -5040,7 +5079,7 @@
     </row>
     <row r="17" spans="1:255" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -5299,7 +5338,7 @@
     </row>
     <row r="18" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -5315,7 +5354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:IV30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleSheetLayoutView="10" workbookViewId="0"/>
@@ -5641,24 +5680,24 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -6445,7 +6484,7 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>
@@ -6978,10 +7017,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D14" s="19"/>
     </row>
@@ -6990,10 +7029,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>50</v>
       </c>
       <c r="D15" s="19"/>
     </row>
@@ -7005,7 +7044,7 @@
     </row>
     <row r="17" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:255" x14ac:dyDescent="0.35">
@@ -7013,31 +7052,31 @@
         <v>19</v>
       </c>
       <c r="B18" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="D18" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="E18" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="F18" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="G18" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="H18" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="I18" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="36" t="s">
+      <c r="J18" s="36" t="s">
         <v>44</v>
-      </c>
-      <c r="J18" s="36" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:255" x14ac:dyDescent="0.35">
@@ -7045,29 +7084,29 @@
         <v>22</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="40" t="s">
+      <c r="G19" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="37" t="s">
+      <c r="H19" s="37" t="s">
         <v>56</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>57</v>
       </c>
       <c r="I19" s="41"/>
       <c r="J19" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:255" ht="15" x14ac:dyDescent="0.35">
@@ -7078,7 +7117,7 @@
     </row>
     <row r="21" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:255" x14ac:dyDescent="0.35">
@@ -7086,10 +7125,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>32</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:255" x14ac:dyDescent="0.35">
@@ -7097,10 +7136,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>35</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:255" x14ac:dyDescent="0.35">
@@ -7108,7 +7147,7 @@
     </row>
     <row r="26" spans="1:255" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -7367,7 +7406,7 @@
     </row>
     <row r="27" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:255" x14ac:dyDescent="0.35">
@@ -7375,12 +7414,12 @@
         <v>23</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A29" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>22</v>
@@ -7388,10 +7427,10 @@
     </row>
     <row r="30" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A30" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -7407,7 +7446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:IV36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleSheetLayoutView="10" workbookViewId="0"/>
@@ -7733,80 +7772,80 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:256" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:256" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>92</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -8593,7 +8632,7 @@
     </row>
     <row r="11" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A11" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>22</v>
@@ -9126,10 +9165,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D15" s="19"/>
     </row>
@@ -9138,32 +9177,32 @@
         <v>1</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="19"/>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="19"/>
     </row>
@@ -9175,39 +9214,39 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="D21" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="E21" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="F21" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="G21" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="H21" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="I21" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="J21" s="36" t="s">
         <v>44</v>
-      </c>
-      <c r="J21" s="36" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -9215,29 +9254,29 @@
         <v>22</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="40" t="s">
+      <c r="G22" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="37" t="s">
+      <c r="H22" s="37" t="s">
         <v>56</v>
-      </c>
-      <c r="H22" s="37" t="s">
-        <v>57</v>
       </c>
       <c r="I22" s="41"/>
       <c r="J22" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -9248,7 +9287,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -9256,21 +9295,21 @@
         <v>19</v>
       </c>
       <c r="B25" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>32</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -9278,7 +9317,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -9286,31 +9325,31 @@
         <v>19</v>
       </c>
       <c r="B29" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="D29" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="E29" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="F29" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="G29" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="H29" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="I29" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="I29" s="36" t="s">
+      <c r="J29" s="36" t="s">
         <v>44</v>
-      </c>
-      <c r="J29" s="36" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -9318,29 +9357,29 @@
         <v>22</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E30" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="37" t="s">
+      <c r="H30" s="37" t="s">
         <v>56</v>
-      </c>
-      <c r="H30" s="37" t="s">
-        <v>57</v>
       </c>
       <c r="I30" s="41"/>
       <c r="J30" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -9351,7 +9390,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:255" x14ac:dyDescent="0.35">
@@ -9359,10 +9398,10 @@
         <v>19</v>
       </c>
       <c r="B33" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="36" t="s">
         <v>32</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:255" x14ac:dyDescent="0.35">
@@ -9370,15 +9409,15 @@
         <v>22</v>
       </c>
       <c r="B34" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>35</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:255" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -9648,7 +9687,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:IV18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleSheetLayoutView="10" workbookViewId="0"/>
@@ -9974,22 +10013,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -10520,7 +10559,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -10778,13 +10817,13 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -11042,7 +11081,7 @@
     </row>
     <row r="11" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:256" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
@@ -11331,7 +11370,7 @@
     </row>
     <row r="17" spans="1:255" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -11590,7 +11629,7 @@
     </row>
     <row r="18" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>